<commit_message>
HypothyroidismAdd file is added
</commit_message>
<xml_diff>
--- a/src/test/resources/RecipeTestData.xlsx
+++ b/src/test/resources/RecipeTestData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1738" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3091" uniqueCount="414">
   <si>
     <t>RecipeID</t>
   </si>
@@ -1251,6 +1251,9 @@
   </si>
   <si>
     <t>Accompaniments Penne with Spinach in Low Calorie White Sauce Whole Wheat Pasta in Low Calorie White Sauce Whole Wheat Spaghetti with Spinach Dumplings in Pumpkin Sauce Nutrient values (Abbrv) per serving Energy 68 cal Protein 2.1 g Carbohydrates 14.9 g Fiber 2.9 g Fat 0.3 g Cholesterol 0 mg Sodium 15 mg Click here to view calories for Rajma Cucumber and Carrot Salad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCOS </t>
   </si>
 </sst>
 </file>
@@ -1365,7 +1368,7 @@
         <v>18</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>20</v>
+        <v>413</v>
       </c>
       <c r="K2" t="s" s="0">
         <v>11</v>
@@ -1505,7 +1508,7 @@
         <v>51</v>
       </c>
       <c r="J6" t="s" s="0">
-        <v>20</v>
+        <v>413</v>
       </c>
       <c r="K6" t="s" s="0">
         <v>44</v>
@@ -2135,7 +2138,7 @@
         <v>176</v>
       </c>
       <c r="J24" t="s" s="0">
-        <v>20</v>
+        <v>413</v>
       </c>
       <c r="K24" t="s" s="0">
         <v>171</v>
@@ -3080,7 +3083,7 @@
         <v>345</v>
       </c>
       <c r="J51" t="s" s="0">
-        <v>20</v>
+        <v>413</v>
       </c>
       <c r="K51" t="s" s="0">
         <v>340</v>

</xml_diff>